<commit_message>
Added WSFC and SQL AG screenshots to the workbook
</commit_message>
<xml_diff>
--- a/WSFC/WSFC-CloudWitness-ResilienceTests.xlsx
+++ b/WSFC/WSFC-CloudWitness-ResilienceTests.xlsx
@@ -5,14 +5,15 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Home\Cybergavin\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="S:\code\misc\WSFC\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9384"/>
   </bookViews>
   <sheets>
-    <sheet name="WSFC RESILIENCE" sheetId="1" r:id="rId1"/>
+    <sheet name="WSFC CLUSTER" sheetId="2" r:id="rId1"/>
+    <sheet name="WSFC RESILIENCE" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="46">
   <si>
     <t>TEST #</t>
   </si>
@@ -1523,12 +1524,15 @@
   <si>
     <t>WSFC (WINDOWS SERVER 2019) WITH CLOUD WITNESS - RESILIENCE TESTS</t>
   </si>
+  <si>
+    <t>SQL AG (CLUSTERED ROLE) ON A WINDOWS 2019 SERVER FAILOVER CLUSTER</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="12" x14ac:knownFonts="1">
+  <fonts count="13" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1621,8 +1625,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="10">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1677,8 +1689,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="12">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -1835,35 +1853,97 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1940,6 +2020,51 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="justify" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="18" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1956,6 +2081,87 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>129541</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>448289</xdr:colOff>
+      <xdr:row>32</xdr:row>
+      <xdr:rowOff>45721</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="0" y="1043941"/>
+          <a:ext cx="6544289" cy="4853940"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>5</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>201118</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>22231</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="6507480" y="1028700"/>
+          <a:ext cx="6495238" cy="5028571"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2221,509 +2427,629 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B0F0"/>
+  </sheetPr>
+  <dimension ref="A1:U4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T47" sqref="T47"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A1" s="35" t="s">
+        <v>45</v>
+      </c>
+      <c r="B1" s="36"/>
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="36"/>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36"/>
+      <c r="J1" s="36"/>
+      <c r="K1" s="36"/>
+      <c r="L1" s="36"/>
+      <c r="M1" s="36"/>
+      <c r="N1" s="36"/>
+      <c r="O1" s="36"/>
+      <c r="P1" s="36"/>
+      <c r="Q1" s="36"/>
+      <c r="R1" s="36"/>
+      <c r="S1" s="36"/>
+      <c r="T1" s="36"/>
+      <c r="U1" s="37"/>
+    </row>
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A2" s="38"/>
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+      <c r="J2" s="39"/>
+      <c r="K2" s="39"/>
+      <c r="L2" s="39"/>
+      <c r="M2" s="39"/>
+      <c r="N2" s="39"/>
+      <c r="O2" s="39"/>
+      <c r="P2" s="39"/>
+      <c r="Q2" s="39"/>
+      <c r="R2" s="39"/>
+      <c r="S2" s="39"/>
+      <c r="T2" s="39"/>
+      <c r="U2" s="40"/>
+    </row>
+    <row r="3" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A3" s="38"/>
+      <c r="B3" s="39"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
+      <c r="G3" s="39"/>
+      <c r="H3" s="39"/>
+      <c r="I3" s="39"/>
+      <c r="J3" s="39"/>
+      <c r="K3" s="39"/>
+      <c r="L3" s="39"/>
+      <c r="M3" s="39"/>
+      <c r="N3" s="39"/>
+      <c r="O3" s="39"/>
+      <c r="P3" s="39"/>
+      <c r="Q3" s="39"/>
+      <c r="R3" s="39"/>
+      <c r="S3" s="39"/>
+      <c r="T3" s="39"/>
+      <c r="U3" s="40"/>
+    </row>
+    <row r="4" spans="1:21" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A4" s="41"/>
+      <c r="B4" s="42"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="42"/>
+      <c r="I4" s="42"/>
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="42"/>
+      <c r="N4" s="42"/>
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="42"/>
+      <c r="S4" s="42"/>
+      <c r="T4" s="42"/>
+      <c r="U4" s="43"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:U4"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <sheetPr>
+    <tabColor rgb="FF00B050"/>
+  </sheetPr>
   <dimension ref="A1:L29"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="H64" sqref="H64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="8.44140625" customWidth="1"/>
-    <col min="2" max="2" width="31.77734375" style="34" customWidth="1"/>
-    <col min="3" max="3" width="24.44140625" style="34" customWidth="1"/>
-    <col min="4" max="4" width="24.6640625" style="34" customWidth="1"/>
-    <col min="5" max="6" width="25.21875" style="34" customWidth="1"/>
-    <col min="7" max="7" width="52.6640625" style="34" customWidth="1"/>
+    <col min="2" max="2" width="31.77734375" style="28" customWidth="1"/>
+    <col min="3" max="3" width="24.44140625" style="28" customWidth="1"/>
+    <col min="4" max="4" width="24.6640625" style="28" customWidth="1"/>
+    <col min="5" max="6" width="25.21875" style="28" customWidth="1"/>
+    <col min="7" max="7" width="52.6640625" style="28" customWidth="1"/>
     <col min="8" max="8" width="8.44140625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
+      <c r="A1" s="29" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s">
+      <c r="B1" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="C1" s="30"/>
+      <c r="D1" s="30"/>
+      <c r="E1" s="30"/>
+      <c r="F1" s="30"/>
+      <c r="G1" s="30"/>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
-      <c r="A2" s="2"/>
-      <c r="B2" s="4"/>
-      <c r="C2" s="5" t="s">
+      <c r="A2" s="29"/>
+      <c r="B2" s="2"/>
+      <c r="C2" s="31" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="5"/>
-      <c r="E2" s="6" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="32" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="6"/>
-      <c r="G2" s="7" t="s">
+      <c r="F2" s="32"/>
+      <c r="G2" s="33" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="4" t="s">
+      <c r="A3" s="29"/>
+      <c r="B3" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="4" t="s">
+      <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="4" t="s">
+      <c r="D3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="4" t="s">
+      <c r="E3" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="F3" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="G3" s="8"/>
+      <c r="G3" s="34"/>
     </row>
     <row r="4" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A4" s="9">
+      <c r="A4" s="3">
         <v>1</v>
       </c>
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="12"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="12"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="6"/>
       <c r="G4" s="1" t="s">
         <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A5" s="9">
+      <c r="A5" s="3">
         <v>2</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="11" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="12"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="12"/>
+      <c r="D5" s="6"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="6"/>
       <c r="G5" s="1" t="s">
         <v>12</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A6" s="9">
+      <c r="A6" s="3">
         <v>3</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="C6" s="11" t="s">
+      <c r="C6" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="13"/>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12"/>
+      <c r="D6" s="7"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
       <c r="G6" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A7" s="9">
+      <c r="A7" s="3">
         <v>4</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="11" t="s">
+      <c r="C7" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="13"/>
-      <c r="E7" s="12"/>
-      <c r="F7" s="12"/>
+      <c r="D7" s="7"/>
+      <c r="E7" s="6"/>
+      <c r="F7" s="6"/>
       <c r="G7" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A8" s="9">
+      <c r="A8" s="3">
         <v>5</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="C8" s="11" t="s">
+      <c r="C8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="13"/>
-      <c r="E8" s="12"/>
-      <c r="F8" s="12"/>
+      <c r="D8" s="7"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
       <c r="G8" s="1" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A9" s="9">
+      <c r="A9" s="3">
         <v>6</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="14" t="s">
+      <c r="C9" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="12"/>
-      <c r="E9" s="12"/>
-      <c r="F9" s="12"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="6"/>
       <c r="G9" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A10" s="9">
+      <c r="A10" s="3">
         <v>7</v>
       </c>
-      <c r="B10" s="15" t="s">
+      <c r="B10" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="14" t="s">
+      <c r="C10" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="12"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="12"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
       <c r="G10" s="1" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A11" s="9">
+      <c r="A11" s="3">
         <v>8</v>
       </c>
-      <c r="B11" s="15" t="s">
+      <c r="B11" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C11" s="12"/>
-      <c r="D11" s="14" t="s">
+      <c r="C11" s="6"/>
+      <c r="D11" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E11" s="12"/>
-      <c r="F11" s="12"/>
+      <c r="E11" s="6"/>
+      <c r="F11" s="6"/>
       <c r="G11" s="1" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A12" s="9">
+      <c r="A12" s="3">
         <v>9</v>
       </c>
-      <c r="B12" s="15" t="s">
+      <c r="B12" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="C12" s="14" t="s">
+      <c r="C12" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="14"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="12"/>
+      <c r="D12" s="8"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
       <c r="G12" s="1" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A13" s="9">
+      <c r="A13" s="3">
         <v>10</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C13" s="14" t="s">
+      <c r="C13" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D13" s="14"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="12"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="6"/>
+      <c r="F13" s="6"/>
       <c r="G13" s="1" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A14" s="9">
+      <c r="A14" s="3">
         <v>11</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C14" s="11" t="s">
+      <c r="C14" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="16"/>
-      <c r="E14" s="17"/>
-      <c r="F14" s="12"/>
+      <c r="D14" s="10"/>
+      <c r="E14" s="11"/>
+      <c r="F14" s="6"/>
       <c r="G14" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A15" s="9">
+      <c r="A15" s="3">
         <v>12</v>
       </c>
-      <c r="B15" s="15" t="s">
+      <c r="B15" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C15" s="14" t="s">
+      <c r="C15" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="12"/>
-      <c r="E15" s="12"/>
-      <c r="F15" s="12"/>
+      <c r="D15" s="6"/>
+      <c r="E15" s="6"/>
+      <c r="F15" s="6"/>
       <c r="G15" s="1" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="9">
+      <c r="A16" s="3">
         <v>13</v>
       </c>
-      <c r="B16" s="15" t="s">
+      <c r="B16" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="C16" s="12"/>
-      <c r="D16" s="18" t="s">
+      <c r="C16" s="6"/>
+      <c r="D16" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="E16" s="13"/>
-      <c r="F16" s="12"/>
+      <c r="E16" s="7"/>
+      <c r="F16" s="6"/>
       <c r="G16" s="1" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="17" spans="1:12" ht="130.80000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A17" s="9">
+      <c r="A17" s="3">
         <v>14</v>
       </c>
-      <c r="B17" s="15" t="s">
+      <c r="B17" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="16"/>
-      <c r="D17" s="19" t="s">
+      <c r="C17" s="10"/>
+      <c r="D17" s="13" t="s">
         <v>11</v>
       </c>
-      <c r="E17" s="20"/>
-      <c r="F17" s="12"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="6"/>
       <c r="G17" s="1" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="18" spans="1:12" ht="130.19999999999999" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A18" s="9">
+      <c r="A18" s="3">
         <v>15</v>
       </c>
-      <c r="B18" s="15" t="s">
+      <c r="B18" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C18" s="14" t="s">
+      <c r="C18" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="12"/>
-      <c r="F18" s="12"/>
+      <c r="D18" s="15"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
       <c r="G18" s="1" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="19" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A19" s="9">
+      <c r="A19" s="3">
         <v>16</v>
       </c>
-      <c r="B19" s="15" t="s">
+      <c r="B19" s="9" t="s">
         <v>30</v>
       </c>
-      <c r="C19" s="13"/>
-      <c r="D19" s="14" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E19" s="12"/>
-      <c r="F19" s="12"/>
+      <c r="E19" s="6"/>
+      <c r="F19" s="6"/>
       <c r="G19" s="1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="20" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A20" s="9">
+      <c r="A20" s="3">
         <v>17</v>
       </c>
-      <c r="B20" s="15" t="s">
+      <c r="B20" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="12"/>
-      <c r="D20" s="12"/>
-      <c r="E20" s="14" t="s">
+      <c r="C20" s="6"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="F20" s="12"/>
+      <c r="F20" s="6"/>
       <c r="G20" s="1" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="21" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A21" s="9">
+      <c r="A21" s="3">
         <v>18</v>
       </c>
-      <c r="B21" s="15" t="s">
+      <c r="B21" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C21" s="14" t="s">
+      <c r="C21" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="12"/>
-      <c r="E21" s="13"/>
-      <c r="F21" s="12"/>
+      <c r="D21" s="6"/>
+      <c r="E21" s="7"/>
+      <c r="F21" s="6"/>
       <c r="G21" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A22" s="9">
+      <c r="A22" s="3">
         <v>19</v>
       </c>
-      <c r="B22" s="15" t="s">
+      <c r="B22" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C22" s="12"/>
-      <c r="D22" s="11" t="s">
+      <c r="C22" s="6"/>
+      <c r="D22" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="E22" s="13"/>
-      <c r="F22" s="12"/>
+      <c r="E22" s="7"/>
+      <c r="F22" s="6"/>
       <c r="G22" s="1" t="s">
         <v>35</v>
       </c>
     </row>
     <row r="23" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A23" s="9">
+      <c r="A23" s="3">
         <v>20</v>
       </c>
-      <c r="B23" s="15" t="s">
+      <c r="B23" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C23" s="12"/>
-      <c r="D23" s="22" t="s">
+      <c r="C23" s="6"/>
+      <c r="D23" s="16" t="s">
         <v>11</v>
       </c>
-      <c r="E23" s="23"/>
-      <c r="F23" s="12"/>
+      <c r="E23" s="17"/>
+      <c r="F23" s="6"/>
       <c r="G23" s="1" t="s">
         <v>36</v>
       </c>
     </row>
     <row r="24" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A24" s="9">
+      <c r="A24" s="3">
         <v>21</v>
       </c>
-      <c r="B24" s="15" t="s">
+      <c r="B24" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C24" s="12"/>
-      <c r="D24" s="24" t="s">
+      <c r="C24" s="6"/>
+      <c r="D24" s="18" t="s">
         <v>11</v>
       </c>
-      <c r="E24" s="12"/>
-      <c r="F24" s="12"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
       <c r="G24" s="1" t="s">
         <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:12" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A25" s="9">
+      <c r="A25" s="3">
         <v>22</v>
       </c>
-      <c r="B25" s="15" t="s">
+      <c r="B25" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="C25" s="25" t="s">
+      <c r="C25" s="19" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="25"/>
-      <c r="E25" s="12"/>
-      <c r="F25" s="12"/>
+      <c r="D25" s="19"/>
+      <c r="E25" s="6"/>
+      <c r="F25" s="6"/>
       <c r="G25" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L25" s="26"/>
+      <c r="L25" s="20"/>
     </row>
     <row r="26" spans="1:12" ht="130.19999999999999" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="9">
+      <c r="A26" s="3">
         <v>23</v>
       </c>
-      <c r="B26" s="27" t="s">
+      <c r="B26" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="C26" s="28" t="s">
+      <c r="C26" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="29"/>
-      <c r="E26" s="30"/>
-      <c r="F26" s="31"/>
+      <c r="D26" s="23"/>
+      <c r="E26" s="24"/>
+      <c r="F26" s="25"/>
       <c r="G26" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:12" ht="130.19999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="9">
+      <c r="A27" s="3">
         <v>24</v>
       </c>
-      <c r="B27" s="32" t="s">
+      <c r="B27" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C27" s="11"/>
-      <c r="D27" s="12"/>
-      <c r="E27" s="33" t="s">
+      <c r="C27" s="5"/>
+      <c r="D27" s="6"/>
+      <c r="E27" s="27" t="s">
         <v>11</v>
       </c>
-      <c r="F27" s="31"/>
+      <c r="F27" s="25"/>
       <c r="G27" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="28" spans="1:12" ht="144.6" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="9">
+      <c r="A28" s="3">
         <v>25</v>
       </c>
-      <c r="B28" s="27" t="s">
+      <c r="B28" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="C28" s="28" t="s">
+      <c r="C28" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="29"/>
-      <c r="E28" s="30"/>
-      <c r="F28" s="31"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="25"/>
       <c r="G28" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="29" spans="1:12" ht="129.6" x14ac:dyDescent="0.3">
-      <c r="A29" s="9">
+      <c r="A29" s="3">
         <v>26</v>
       </c>
-      <c r="B29" s="32" t="s">
+      <c r="B29" s="26" t="s">
         <v>28</v>
       </c>
-      <c r="C29" s="11"/>
-      <c r="D29" s="12"/>
-      <c r="E29" s="18" t="s">
+      <c r="C29" s="5"/>
+      <c r="D29" s="6"/>
+      <c r="E29" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="F29" s="31"/>
+      <c r="F29" s="25"/>
       <c r="G29" s="1" t="s">
         <v>43</v>
       </c>

</xml_diff>